<commit_message>
Se agregaron los códigos de HomePage
</commit_message>
<xml_diff>
--- a/Documentos/Normalizacion Aumento Espacio.xlsx
+++ b/Documentos/Normalizacion Aumento Espacio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\GitHub\TechOrganizeContenido\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{317E05EF-A5E0-4E49-BC9A-8B47F081E4BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90E5783-8401-4942-9AEE-2A793209DB21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="99">
   <si>
     <t>Tabla sin Normalizar</t>
   </si>
@@ -268,13 +268,67 @@
   </si>
   <si>
     <t>Solicitud/Aumento</t>
+  </si>
+  <si>
+    <t>ID_Archivo</t>
+  </si>
+  <si>
+    <t>Nombre Archivo</t>
+  </si>
+  <si>
+    <t>Tipo Archivo</t>
+  </si>
+  <si>
+    <t>Fecha Subida</t>
+  </si>
+  <si>
+    <t>Peso Archivo</t>
+  </si>
+  <si>
+    <t>Rol</t>
+  </si>
+  <si>
+    <t>Guia Js</t>
+  </si>
+  <si>
+    <t>Docx.</t>
+  </si>
+  <si>
+    <t>396KB</t>
+  </si>
+  <si>
+    <t>ID_Reporte</t>
+  </si>
+  <si>
+    <t>Nombre Usuario</t>
+  </si>
+  <si>
+    <t>Fecha Descarga</t>
+  </si>
+  <si>
+    <t>Fecha Reporte</t>
+  </si>
+  <si>
+    <t>Estado (En Revision/Revisado)</t>
+  </si>
+  <si>
+    <t>Revisado</t>
+  </si>
+  <si>
+    <t>Jhon Freddy Faragin Cortez</t>
+  </si>
+  <si>
+    <t>Virus/Error</t>
+  </si>
+  <si>
+    <t>Ninguno</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -313,12 +367,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Docs-Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="11">
@@ -383,7 +431,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -474,11 +522,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -607,8 +685,27 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -633,7 +730,7 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>2581275</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>94</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="361950" cy="342900"/>
@@ -650,7 +747,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6745061" y="15845518"/>
+          <a:off x="6745061" y="22349732"/>
           <a:ext cx="361950" cy="342900"/>
           <a:chOff x="2607550" y="644225"/>
           <a:chExt cx="1165800" cy="1063500"/>
@@ -694,7 +791,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1304925</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>94</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="438150" cy="342900"/>
@@ -711,7 +808,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8094889" y="15845518"/>
+          <a:off x="8094889" y="22349732"/>
           <a:ext cx="438150" cy="342900"/>
           <a:chOff x="2699575" y="10225"/>
           <a:chExt cx="1441800" cy="1196400"/>
@@ -755,7 +852,7 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1352550</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>94</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="438150" cy="342900"/>
@@ -772,7 +869,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9911443" y="15845518"/>
+          <a:off x="10578193" y="22349732"/>
           <a:ext cx="438150" cy="342900"/>
           <a:chOff x="378350" y="10225"/>
           <a:chExt cx="1083900" cy="818100"/>
@@ -1015,8 +1112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1024,13 +1121,13 @@
     <col min="1" max="1" width="19.7109375" customWidth="1"/>
     <col min="2" max="2" width="42.5703125" customWidth="1"/>
     <col min="3" max="3" width="39.28515625" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="36.5703125" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" customWidth="1"/>
     <col min="6" max="6" width="28.42578125" customWidth="1"/>
-    <col min="7" max="7" width="39.5703125" customWidth="1"/>
+    <col min="7" max="7" width="35.7109375" customWidth="1"/>
     <col min="8" max="8" width="26" customWidth="1"/>
     <col min="9" max="9" width="25.7109375" customWidth="1"/>
-    <col min="10" max="10" width="38.140625" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" customWidth="1"/>
     <col min="11" max="11" width="20.42578125" customWidth="1"/>
     <col min="12" max="12" width="22.5703125" customWidth="1"/>
     <col min="13" max="13" width="26.7109375" customWidth="1"/>
@@ -1050,7 +1147,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="5"/>
-      <c r="J1" s="6"/>
+      <c r="J1" s="5"/>
       <c r="K1" s="6"/>
       <c r="L1" s="7"/>
       <c r="M1" s="8"/>
@@ -1085,7 +1182,9 @@
       <c r="I2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="12"/>
+      <c r="J2" s="10" t="s">
+        <v>86</v>
+      </c>
       <c r="K2" s="13"/>
       <c r="L2" s="12"/>
       <c r="M2" s="12"/>
@@ -1119,7 +1218,9 @@
       <c r="I3" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="17"/>
+      <c r="J3" s="16" t="s">
+        <v>72</v>
+      </c>
       <c r="K3" s="17"/>
       <c r="L3" s="17"/>
       <c r="M3" s="17"/>
@@ -1153,7 +1254,9 @@
       <c r="I4" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="17"/>
+      <c r="J4" s="20" t="s">
+        <v>72</v>
+      </c>
       <c r="K4" s="17"/>
       <c r="L4" s="17"/>
       <c r="M4" s="17"/>
@@ -1187,7 +1290,9 @@
       <c r="I5" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="J5" s="17"/>
+      <c r="J5" s="16" t="s">
+        <v>72</v>
+      </c>
       <c r="K5" s="17"/>
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
@@ -1221,7 +1326,9 @@
       <c r="I6" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="17"/>
+      <c r="J6" s="20" t="s">
+        <v>72</v>
+      </c>
       <c r="K6" s="17"/>
       <c r="L6" s="17"/>
       <c r="M6" s="17"/>
@@ -1255,7 +1362,9 @@
       <c r="I7" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="J7" s="17"/>
+      <c r="J7" s="16" t="s">
+        <v>72</v>
+      </c>
       <c r="K7" s="17"/>
       <c r="L7" s="17"/>
       <c r="M7" s="17"/>
@@ -1289,7 +1398,9 @@
       <c r="I8" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="J8" s="8"/>
+      <c r="J8" s="20" t="s">
+        <v>72</v>
+      </c>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
@@ -1300,983 +1411,1022 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
+      <c r="G10" s="57"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
+      <c r="A11" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="54" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="G11" s="52"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
+      <c r="A12" s="14">
+        <v>1</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" s="16">
+        <v>44701</v>
+      </c>
+      <c r="E12" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" s="59" t="s">
+        <v>98</v>
+      </c>
+      <c r="G12" s="53"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="21"/>
+      <c r="G13" s="57"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
     </row>
-    <row r="15" spans="1:17" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A15" s="22"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N15" s="23"/>
       <c r="O15" s="23"/>
       <c r="P15" s="23"/>
       <c r="Q15" s="23"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" s="54" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="14">
         <v>1</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B21" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="16">
+        <v>45066</v>
+      </c>
+      <c r="E21" s="55" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E24" s="52"/>
+    </row>
+    <row r="25" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E25" s="53"/>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" s="54" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="14">
+        <v>1</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" s="16">
+        <v>44859</v>
+      </c>
+      <c r="D30" s="56" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:13" ht="57" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A45" s="22"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
+    </row>
+    <row r="46" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C46" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D46" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E46" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F46" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G46" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H46" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="I16" s="10" t="s">
+      <c r="I46" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J16" s="10" t="s">
+      <c r="J46" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="K16" s="10" t="s">
+      <c r="K46" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="L16" s="10" t="s">
+      <c r="L46" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="M16" s="24" t="s">
+      <c r="M46" s="24" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+    <row r="47" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="14">
+      <c r="B47" s="14">
         <v>80830111</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C47" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D47" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E47" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F47" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G47" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="H47" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I17" s="15">
+      <c r="I47" s="15">
         <v>6900</v>
       </c>
-      <c r="J17" s="14" t="s">
+      <c r="J47" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="K17" s="14">
+      <c r="K47" s="14">
         <v>1</v>
       </c>
-      <c r="L17" s="16">
+      <c r="L47" s="16">
         <v>45037</v>
       </c>
-      <c r="M17" s="16">
+      <c r="M47" s="16">
         <v>45067</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
+    <row r="48" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B48" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C48" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="18" t="s">
+      <c r="D48" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="E18" s="18" t="s">
+      <c r="E48" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="F18" s="18" t="s">
+      <c r="F48" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="G18" s="18" t="s">
+      <c r="G48" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="18" t="s">
+      <c r="H48" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="I18" s="19">
+      <c r="I48" s="19">
         <v>10900</v>
       </c>
-      <c r="J18" s="18" t="s">
+      <c r="J48" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="K18" s="18">
+      <c r="K48" s="18">
         <v>2</v>
       </c>
-      <c r="L18" s="20">
+      <c r="L48" s="20">
         <v>45062</v>
       </c>
-      <c r="M18" s="20">
+      <c r="M48" s="20">
         <v>45093</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+    <row r="49" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="14">
+      <c r="B49" s="14">
         <v>1033814672</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C49" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D49" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E49" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F49" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="G49" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="H19" s="14" t="s">
+      <c r="H49" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="I19" s="15">
+      <c r="I49" s="15">
         <v>17900</v>
       </c>
-      <c r="J19" s="14" t="s">
+      <c r="J49" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="K19" s="14">
+      <c r="K49" s="14">
         <v>3</v>
       </c>
-      <c r="L19" s="16" t="s">
+      <c r="L49" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="M19" s="16">
+      <c r="M49" s="16">
         <v>45067</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
+    <row r="50" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B50" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C50" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D50" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E50" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="F20" s="18" t="s">
+      <c r="F50" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="G20" s="18" t="s">
+      <c r="G50" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="H20" s="18" t="s">
+      <c r="H50" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="I20" s="19">
+      <c r="I50" s="19">
         <v>6900</v>
       </c>
-      <c r="J20" s="18" t="s">
+      <c r="J50" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="K20" s="18">
+      <c r="K50" s="18">
         <v>1</v>
       </c>
-      <c r="L20" s="20">
+      <c r="L50" s="20">
         <v>45062</v>
       </c>
-      <c r="M20" s="20">
+      <c r="M50" s="20">
         <v>45093</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+    <row r="51" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="14">
+      <c r="B51" s="14">
         <v>24685716</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C51" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D51" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E51" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F51" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="G51" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="H21" s="14" t="s">
+      <c r="H51" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="I21" s="15">
+      <c r="I51" s="15">
         <v>10900</v>
       </c>
-      <c r="J21" s="14" t="s">
+      <c r="J51" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="K21" s="14">
+      <c r="K51" s="14">
         <v>2</v>
       </c>
-      <c r="L21" s="16">
+      <c r="L51" s="16">
         <v>45037</v>
       </c>
-      <c r="M21" s="16">
+      <c r="M51" s="16">
         <v>45067</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
+    <row r="52" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="18">
+      <c r="B52" s="18">
         <v>7032502146</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C52" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D52" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="E52" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="F22" s="18" t="s">
+      <c r="F52" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="G22" s="18" t="s">
+      <c r="G52" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="H22" s="18" t="s">
+      <c r="H52" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="I22" s="19">
+      <c r="I52" s="19">
         <v>6900</v>
       </c>
-      <c r="J22" s="18" t="s">
+      <c r="J52" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="K22" s="18">
+      <c r="K52" s="18">
         <v>1</v>
       </c>
-      <c r="L22" s="20">
+      <c r="L52" s="20">
         <v>45062</v>
       </c>
-      <c r="M22" s="20">
+      <c r="M52" s="20">
         <v>45093</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
-    </row>
-    <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
-    </row>
-    <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
-    </row>
-    <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
-    </row>
-    <row r="27" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="21"/>
-    </row>
-    <row r="28" spans="1:13" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="4" t="s">
+    <row r="53" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="21"/>
+    </row>
+    <row r="54" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="21"/>
+    </row>
+    <row r="55" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="21"/>
+    </row>
+    <row r="56" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="21"/>
+    </row>
+    <row r="57" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="21"/>
+    </row>
+    <row r="58" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="22"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="23"/>
-    </row>
-    <row r="29" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A29" s="25"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="27" t="s">
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="23"/>
+    </row>
+    <row r="59" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A59" s="25"/>
+      <c r="B59" s="26"/>
+      <c r="C59" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="D29" s="28"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="23"/>
-    </row>
-    <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
+      <c r="D59" s="28"/>
+      <c r="E59" s="26"/>
+      <c r="F59" s="29"/>
+      <c r="G59" s="23"/>
+    </row>
+    <row r="60" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B60" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C60" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D60" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E30" s="24" t="s">
+      <c r="E60" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="F30" s="11" t="s">
+      <c r="F60" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14">
+    <row r="61" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="14">
         <v>80830111</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B61" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C61" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D61" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E61" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="F31" s="14" t="s">
+      <c r="F61" s="14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="18" t="s">
+    <row r="62" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B62" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C62" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D32" s="18" t="s">
+      <c r="D62" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="E32" s="31" t="s">
+      <c r="E62" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="F32" s="18" t="s">
+      <c r="F62" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14">
+    <row r="63" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="14">
         <v>1033814672</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B63" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C63" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D63" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="E33" s="30" t="s">
+      <c r="E63" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="F33" s="14" t="s">
+      <c r="F63" s="14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="18" t="s">
+    <row r="64" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B64" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C64" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="D34" s="18" t="s">
+      <c r="D64" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="E34" s="31" t="s">
+      <c r="E64" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="F34" s="18" t="s">
+      <c r="F64" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="14">
+    <row r="65" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="14">
         <v>24685716</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B65" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C65" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="14" t="s">
+      <c r="D65" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="E35" s="30" t="s">
+      <c r="E65" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="F35" s="14" t="s">
+      <c r="F65" s="14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="18">
+    <row r="66" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="18">
         <v>7032502146</v>
       </c>
-      <c r="B36" s="32" t="s">
+      <c r="B66" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="32" t="s">
+      <c r="C66" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="D36" s="32" t="s">
+      <c r="D66" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="E36" s="18" t="s">
+      <c r="E66" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="F36" s="18" t="s">
+      <c r="F66" s="18" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A37" s="21"/>
-      <c r="B37" s="23"/>
-      <c r="C37" s="33"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
-    </row>
-    <row r="38" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A38" s="25"/>
-      <c r="B38" s="34" t="s">
+    <row r="67" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A67" s="21"/>
+      <c r="B67" s="23"/>
+      <c r="C67" s="33"/>
+      <c r="D67" s="23"/>
+      <c r="E67" s="23"/>
+    </row>
+    <row r="68" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A68" s="25"/>
+      <c r="B68" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="C38" s="35"/>
-      <c r="D38" s="23"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="34" t="s">
+      <c r="C68" s="35"/>
+      <c r="D68" s="23"/>
+      <c r="E68" s="25"/>
+      <c r="F68" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="G38" s="36"/>
-      <c r="K38" s="37"/>
-      <c r="L38" s="38"/>
-      <c r="M38" s="39"/>
-    </row>
-    <row r="39" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
+      <c r="G68" s="36"/>
+      <c r="K68" s="37"/>
+      <c r="L68" s="38"/>
+      <c r="M68" s="39"/>
+    </row>
+    <row r="69" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B69" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C69" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="E69" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F39" s="10" t="s">
+      <c r="F69" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="G39" s="24" t="s">
+      <c r="G69" s="24" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="14">
+    <row r="70" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="14">
         <v>1</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B70" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="15">
+      <c r="C70" s="15">
         <v>6900</v>
       </c>
-      <c r="E40" s="14" t="s">
+      <c r="E70" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F40" s="16">
+      <c r="F70" s="16">
         <v>45037</v>
       </c>
-      <c r="G40" s="16">
+      <c r="G70" s="16">
         <v>45067</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="18">
+    <row r="71" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="18">
         <v>2</v>
       </c>
-      <c r="B41" s="18" t="s">
+      <c r="B71" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C41" s="19">
+      <c r="C71" s="19">
         <v>10900</v>
       </c>
-      <c r="E41" s="18" t="s">
+      <c r="E71" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="F41" s="20">
+      <c r="F71" s="20">
         <v>45062</v>
       </c>
-      <c r="G41" s="20">
+      <c r="G71" s="20">
         <v>45093</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="14">
+    <row r="72" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="14">
         <v>3</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="B72" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C42" s="15">
+      <c r="C72" s="15">
         <v>17900</v>
       </c>
-      <c r="E42" s="14" t="s">
+      <c r="E72" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="F42" s="16" t="s">
+      <c r="F72" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="G42" s="16">
+      <c r="G72" s="16">
         <v>45067</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="18">
+    <row r="73" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="18">
         <v>1</v>
       </c>
-      <c r="B43" s="18" t="s">
+      <c r="B73" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="19">
+      <c r="C73" s="19">
         <v>6900</v>
       </c>
-      <c r="E43" s="18" t="s">
+      <c r="E73" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F43" s="20">
+      <c r="F73" s="20">
         <v>45062</v>
       </c>
-      <c r="G43" s="20">
+      <c r="G73" s="20">
         <v>45093</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="14">
+    <row r="74" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="14">
         <v>2</v>
       </c>
-      <c r="B44" s="14" t="s">
+      <c r="B74" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C44" s="15">
+      <c r="C74" s="15">
         <v>10900</v>
       </c>
-      <c r="E44" s="14" t="s">
+      <c r="E74" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F44" s="16">
+      <c r="F74" s="16">
         <v>45037</v>
       </c>
-      <c r="G44" s="16">
+      <c r="G74" s="16">
         <v>45067</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="18">
+    <row r="75" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="18">
         <v>1</v>
       </c>
-      <c r="B45" s="18" t="s">
+      <c r="B75" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C45" s="19">
+      <c r="C75" s="19">
         <v>6900</v>
       </c>
-      <c r="E45" s="18" t="s">
+      <c r="E75" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F45" s="20">
+      <c r="F75" s="20">
         <v>45062</v>
       </c>
-      <c r="G45" s="20">
+      <c r="G75" s="20">
         <v>45093</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="21"/>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="21"/>
-      <c r="G46" s="21"/>
-    </row>
-    <row r="47" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="22"/>
-      <c r="B47" s="4" t="s">
+    <row r="76" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="21"/>
+      <c r="B76" s="21"/>
+      <c r="C76" s="21"/>
+      <c r="D76" s="21"/>
+      <c r="E76" s="21"/>
+      <c r="F76" s="21"/>
+      <c r="G76" s="21"/>
+    </row>
+    <row r="77" spans="1:13" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="22"/>
+      <c r="B77" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C47" s="40"/>
-      <c r="D47" s="23"/>
-      <c r="E47" s="41"/>
-      <c r="F47" s="23"/>
-      <c r="G47" s="21"/>
-    </row>
-    <row r="48" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="21"/>
-      <c r="B48" s="21"/>
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
-      <c r="E48" s="21"/>
-      <c r="F48" s="21"/>
-      <c r="G48" s="21"/>
-    </row>
-    <row r="49" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A49" s="25"/>
-      <c r="B49" s="42" t="s">
+      <c r="C77" s="40"/>
+      <c r="D77" s="23"/>
+      <c r="E77" s="41"/>
+      <c r="F77" s="23"/>
+      <c r="G77" s="21"/>
+    </row>
+    <row r="78" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="21"/>
+      <c r="B78" s="21"/>
+      <c r="C78" s="21"/>
+      <c r="D78" s="21"/>
+      <c r="E78" s="21"/>
+      <c r="F78" s="21"/>
+      <c r="G78" s="21"/>
+    </row>
+    <row r="79" spans="1:13" ht="54" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A79" s="25"/>
+      <c r="B79" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="C49" s="26"/>
-    </row>
-    <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="9" t="s">
+      <c r="C79" s="26"/>
+    </row>
+    <row r="80" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="B80" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C50" s="10" t="s">
+      <c r="C80" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="14">
+    <row r="81" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="14">
         <v>1</v>
       </c>
-      <c r="B51" s="14">
+      <c r="B81" s="14">
         <v>80830111</v>
       </c>
-      <c r="C51" s="14" t="s">
+      <c r="C81" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="18">
+    <row r="82" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="18">
         <v>2</v>
       </c>
-      <c r="B52" s="18" t="s">
+      <c r="B82" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C52" s="18" t="s">
+      <c r="C82" s="18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="14">
+    <row r="83" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="14">
         <v>3</v>
       </c>
-      <c r="B53" s="14">
+      <c r="B83" s="14">
         <v>1033814672</v>
       </c>
-      <c r="C53" s="14" t="s">
+      <c r="C83" s="14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="18">
+    <row r="84" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="18">
         <v>1</v>
       </c>
-      <c r="B54" s="18" t="s">
+      <c r="B84" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C54" s="43" t="s">
+      <c r="C84" s="43" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="14">
+    <row r="85" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="14">
         <v>2</v>
       </c>
-      <c r="B55" s="14">
+      <c r="B85" s="14">
         <v>24685716</v>
       </c>
-      <c r="C55" s="14" t="s">
+      <c r="C85" s="14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="18">
+    <row r="86" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="18">
         <v>1</v>
       </c>
-      <c r="B56" s="18">
+      <c r="B86" s="18">
         <v>7032502146</v>
       </c>
-      <c r="C56" s="18" t="s">
+      <c r="C86" s="18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="D58" s="44"/>
-      <c r="E58" s="23"/>
-    </row>
-    <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="45"/>
-      <c r="B59" s="46"/>
-      <c r="C59" s="23"/>
-      <c r="D59" s="23"/>
-      <c r="E59" s="23"/>
-      <c r="F59" s="23"/>
-    </row>
-    <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="21"/>
-      <c r="B60" s="21"/>
-      <c r="C60" s="47" t="s">
+    <row r="87" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="D88" s="44"/>
+      <c r="E88" s="23"/>
+    </row>
+    <row r="89" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="45"/>
+      <c r="B89" s="46"/>
+      <c r="C89" s="23"/>
+      <c r="D89" s="23"/>
+      <c r="E89" s="23"/>
+      <c r="F89" s="23"/>
+    </row>
+    <row r="90" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="21"/>
+      <c r="B90" s="21"/>
+      <c r="C90" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="D60" s="48" t="s">
+      <c r="D90" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="E60" s="23"/>
-      <c r="F60" s="23"/>
-    </row>
-    <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="21"/>
-      <c r="B61" s="21"/>
-      <c r="C61" s="49" t="s">
+      <c r="E90" s="23"/>
+      <c r="F90" s="23"/>
+    </row>
+    <row r="91" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="21"/>
+      <c r="B91" s="21"/>
+      <c r="C91" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="D61" s="50" t="s">
+      <c r="D91" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="E61" s="51" t="s">
+      <c r="E91" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="F61" s="50" t="s">
+      <c r="F91" s="50" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="21"/>
-      <c r="C62" s="23"/>
-      <c r="D62" s="23"/>
-      <c r="E62" s="23"/>
-      <c r="F62" s="23"/>
-    </row>
-    <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="21"/>
-      <c r="C63" s="23"/>
-      <c r="D63" s="23"/>
-      <c r="E63" s="23" t="s">
+    <row r="92" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="21"/>
+      <c r="C92" s="23"/>
+      <c r="D92" s="23"/>
+      <c r="E92" s="23"/>
+      <c r="F92" s="23"/>
+    </row>
+    <row r="93" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="21"/>
+      <c r="C93" s="23"/>
+      <c r="D93" s="23"/>
+      <c r="E93" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="F63" s="23"/>
-    </row>
-    <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="21"/>
-      <c r="B64" s="21"/>
-      <c r="C64" s="23"/>
-      <c r="D64" s="21"/>
-      <c r="E64" s="23"/>
-      <c r="F64" s="23"/>
-    </row>
-    <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C65" s="50" t="s">
+      <c r="F93" s="23"/>
+    </row>
+    <row r="94" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="21"/>
+      <c r="B94" s="21"/>
+      <c r="C94" s="23"/>
+      <c r="D94" s="21"/>
+      <c r="E94" s="23"/>
+      <c r="F94" s="23"/>
+    </row>
+    <row r="95" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C95" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="E65" s="48" t="s">
+      <c r="E95" s="48" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C66" s="23"/>
-      <c r="D66" s="23"/>
-      <c r="F66" s="23"/>
-    </row>
-    <row r="67" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C67" s="23"/>
-      <c r="D67" s="50" t="s">
+    <row r="96" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C96" s="23"/>
+      <c r="D96" s="23"/>
+      <c r="F96" s="23"/>
+    </row>
+    <row r="97" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C97" s="23"/>
+      <c r="D97" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="E67" s="23"/>
-      <c r="F67" s="50" t="s">
+      <c r="E97" s="23"/>
+      <c r="F97" s="50" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C68" s="21"/>
-      <c r="D68" s="23"/>
-      <c r="E68" s="23"/>
-      <c r="F68" s="23"/>
-    </row>
-    <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C69" s="23"/>
-      <c r="D69" s="23"/>
-      <c r="F69" s="23"/>
-    </row>
-    <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="23"/>
-      <c r="C70" s="23"/>
-      <c r="D70" s="23"/>
-      <c r="E70" s="23"/>
-      <c r="F70" s="23"/>
-    </row>
-    <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="23"/>
-      <c r="C71" s="23"/>
-      <c r="D71" s="23"/>
-      <c r="E71" s="23"/>
-      <c r="F71" s="23"/>
-    </row>
-    <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="23"/>
-      <c r="C72" s="23"/>
-      <c r="D72" s="23"/>
-      <c r="E72" s="23"/>
-      <c r="F72" s="23"/>
-    </row>
-    <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="23"/>
-      <c r="C73" s="21"/>
-      <c r="D73" s="21"/>
-    </row>
-    <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="23"/>
-      <c r="C74" s="21"/>
-      <c r="D74" s="23"/>
-      <c r="E74" s="23"/>
-      <c r="F74" s="23"/>
-    </row>
-    <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="23"/>
-      <c r="C75" s="23"/>
-      <c r="D75" s="23"/>
-      <c r="E75" s="23"/>
-      <c r="F75" s="23"/>
-    </row>
-    <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="23"/>
-      <c r="C76" s="23"/>
-      <c r="D76" s="23"/>
-      <c r="E76" s="23"/>
-    </row>
-    <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="23"/>
-    </row>
-    <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="23"/>
-    </row>
-    <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="23"/>
-    </row>
-    <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="23"/>
-    </row>
-    <row r="81" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="23"/>
-    </row>
-    <row r="82" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="23"/>
-    </row>
-    <row r="83" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="23"/>
-    </row>
-    <row r="84" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="52"/>
-    </row>
-    <row r="85" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="52"/>
-    </row>
-    <row r="86" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="23"/>
-    </row>
-    <row r="87" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="23"/>
-    </row>
-    <row r="88" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C98" s="21"/>
+      <c r="D98" s="23"/>
+      <c r="E98" s="23"/>
+      <c r="F98" s="23"/>
+    </row>
+    <row r="99" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C99" s="23"/>
+      <c r="D99" s="23"/>
+      <c r="F99" s="23"/>
+    </row>
+    <row r="100" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>